<commit_message>
Added info about seconds.
</commit_message>
<xml_diff>
--- a/Results/2012-03 #1/Results.xlsx
+++ b/Results/2012-03 #1/Results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
   <si>
     <t>Medium set (10.000)</t>
   </si>
@@ -166,6 +166,12 @@
   <si>
     <t>RavenDb returns 128 rows while SisoDb returns the full match of 16668 rows</t>
   </si>
+  <si>
+    <t>All measurements are measured in seconds</t>
+  </si>
+  <si>
+    <t>Numbers are in seconds</t>
+  </si>
 </sst>
 </file>
 
@@ -174,7 +180,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +213,22 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -267,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -291,6 +313,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,10 +621,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K37"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,6 +638,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>25</v>
+      </c>
       <c r="B1" s="12" t="s">
         <v>14</v>
       </c>
@@ -1291,6 +1320,7 @@
         <f>MEDIAN(C28:C30)</f>
         <v>9.9000000000000008E-3</v>
       </c>
+      <c r="D31" s="13"/>
       <c r="F31" s="8">
         <f>MEDIAN(F28:F30)</f>
         <v>4.8280000000000003E-2</v>
@@ -1308,34 +1338,41 @@
         <v>0.43130000000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="9" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="9" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="9" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added info about 128 vs 16668
</commit_message>
<xml_diff>
--- a/Results/2012-03 #1/Results.xlsx
+++ b/Results/2012-03 #1/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
   <si>
     <t>Medium set (10.000)</t>
   </si>
@@ -77,81 +77,6 @@
     <t>**</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">** </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Query trip #1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">** </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>#2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">** </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>#3</t>
-    </r>
-  </si>
-  <si>
     <t>I'm not a skilled RavenDb user, hence my figures for RavenDb could probably be tweaked.</t>
   </si>
   <si>
@@ -161,9 +86,6 @@
     <t>***</t>
   </si>
   <si>
-    <t>RavenDb only returns max 128 rows per default, while SisoDb all matches.</t>
-  </si>
-  <si>
     <t>RavenDb returns 128 rows while SisoDb returns the full match of 16668 rows</t>
   </si>
   <si>
@@ -171,6 +93,15 @@
   </si>
   <si>
     <t>Numbers are in seconds</t>
+  </si>
+  <si>
+    <t>Query trip #1</t>
+  </si>
+  <si>
+    <t>RavenDb returns 128 rows while SisoDb returns the full match of 1668 rows</t>
+  </si>
+  <si>
+    <t>Not fair to compare 128 vs 16668 records</t>
   </si>
 </sst>
 </file>
@@ -236,7 +167,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -258,6 +189,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -289,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -320,6 +263,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,8 +574,8 @@
   </sheetPr>
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +590,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>14</v>
@@ -684,7 +632,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="16" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5">
@@ -791,7 +739,7 @@
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="16" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="5">
@@ -898,7 +846,7 @@
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="5">
@@ -1005,7 +953,7 @@
       <c r="K17" s="3"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="16" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="5">
@@ -1112,7 +1060,7 @@
       <c r="K22" s="3"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B23" s="5">
@@ -1219,8 +1167,8 @@
       <c r="K27" s="3"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>16</v>
+      <c r="A28" s="16" t="s">
+        <v>22</v>
       </c>
       <c r="B28" s="5">
         <v>0.19320000000000001</v>
@@ -1229,6 +1177,9 @@
         <v>5.4300000000000001E-2</v>
       </c>
       <c r="D28" s="10"/>
+      <c r="E28" s="11" t="s">
+        <v>15</v>
+      </c>
       <c r="F28" s="5">
         <v>0.48270000000000002</v>
       </c>
@@ -1237,7 +1188,7 @@
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J28" s="5">
         <v>0.4093</v>
@@ -1248,7 +1199,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="B29" s="5">
         <v>3.5799999999999998E-2</v>
@@ -1257,6 +1208,9 @@
         <v>9.9000000000000008E-3</v>
       </c>
       <c r="D29" s="10"/>
+      <c r="E29" s="11" t="s">
+        <v>15</v>
+      </c>
       <c r="F29" s="5">
         <v>4.8280000000000003E-2</v>
       </c>
@@ -1265,7 +1219,7 @@
       </c>
       <c r="H29" s="10"/>
       <c r="I29" s="11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J29" s="5">
         <v>6.1499999999999999E-2</v>
@@ -1276,7 +1230,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B30" s="5">
         <v>3.3700000000000001E-2</v>
@@ -1285,6 +1239,9 @@
         <v>9.4999999999999998E-3</v>
       </c>
       <c r="D30" s="10"/>
+      <c r="E30" s="11" t="s">
+        <v>15</v>
+      </c>
       <c r="F30" s="5">
         <v>3.5299999999999998E-2</v>
       </c>
@@ -1293,7 +1250,7 @@
       </c>
       <c r="H30" s="10"/>
       <c r="I30" s="11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J30" s="5">
         <v>6.4299999999999996E-2</v>
@@ -1315,6 +1272,9 @@
         <v>9.9000000000000008E-3</v>
       </c>
       <c r="D31" s="13"/>
+      <c r="E31" s="11" t="s">
+        <v>15</v>
+      </c>
       <c r="F31" s="8">
         <f>MEDIAN(F28:F30)</f>
         <v>4.8280000000000003E-2</v>
@@ -1323,19 +1283,27 @@
         <f>MEDIAN(G28:G30)</f>
         <v>4.0599999999999997E-2</v>
       </c>
-      <c r="J31" s="6">
+      <c r="I31" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J31" s="18">
         <f>MEDIAN(J28:J30)</f>
         <v>6.4299999999999996E-2</v>
       </c>
-      <c r="K31" s="8">
+      <c r="K31" s="17">
         <f>MEDIAN(K28:K30)</f>
         <v>0.43130000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J32" s="9" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C33" s="1"/>
     </row>
@@ -1352,25 +1320,25 @@
         <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B36" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" s="9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>